<commit_message>
Cromar's feedback and CB1 factor effects
</commit_message>
<xml_diff>
--- a/data/toothpaste_bf2.xlsx
+++ b/data/toothpaste_bf2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/Math326DoE/Math326_Quarto4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="8_{1530781B-6E7F-4C73-ADF8-9272CFAEB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A8E9306-9881-4694-9335-771B5FCE049C}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="8_{1530781B-6E7F-4C73-ADF8-9272CFAEB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{671CCE9F-02F7-4A53-9903-28EA06FFB3BF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
@@ -2313,7 +2313,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2537,13 +2537,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="27" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="27" fillId="33" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2573,40 +2629,22 @@
     <xf numFmtId="2" fontId="25" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2615,48 +2653,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3002,6 +2998,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3656,12 +3656,12 @@
         <v>58</v>
       </c>
       <c r="K1" s="56"/>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="104" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
     </row>
     <row r="2" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
@@ -3676,12 +3676,12 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="91" t="s">
+      <c r="G2" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
       <c r="L2" s="39" t="s">
         <v>4</v>
       </c>
@@ -4062,12 +4062,12 @@
       <c r="C11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="89" t="s">
+      <c r="L11" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="89"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="89"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="104"/>
     </row>
     <row r="12" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
@@ -4082,12 +4082,12 @@
       <c r="E12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="91" t="s">
+      <c r="G12" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H12" s="91"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
       <c r="L12" s="12" t="s">
         <v>4</v>
       </c>
@@ -4100,12 +4100,12 @@
       <c r="O12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="91" t="s">
+      <c r="Q12" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="R12" s="91"/>
-      <c r="S12" s="91"/>
-      <c r="T12" s="91"/>
+      <c r="R12" s="105"/>
+      <c r="S12" s="105"/>
+      <c r="T12" s="105"/>
     </row>
     <row r="13" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
@@ -4522,12 +4522,12 @@
       <c r="C23" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L23" s="89" t="s">
+      <c r="L23" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="M23" s="89"/>
-      <c r="N23" s="89"/>
-      <c r="O23" s="89"/>
+      <c r="M23" s="104"/>
+      <c r="N23" s="104"/>
+      <c r="O23" s="104"/>
     </row>
     <row r="24" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
@@ -4542,12 +4542,12 @@
       <c r="E24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="91" t="s">
+      <c r="G24" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="91"/>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
       <c r="L24" s="12" t="s">
         <v>4</v>
       </c>
@@ -4560,12 +4560,12 @@
       <c r="O24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="104" t="s">
+      <c r="Q24" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
+      <c r="R24" s="111"/>
+      <c r="S24" s="111"/>
+      <c r="T24" s="111"/>
     </row>
     <row r="25" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
@@ -4751,12 +4751,12 @@
       <c r="C33" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L33" s="89" t="s">
+      <c r="L33" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="M33" s="89"/>
-      <c r="N33" s="89"/>
-      <c r="O33" s="89"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="104"/>
     </row>
     <row r="34" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
@@ -4771,12 +4771,12 @@
       <c r="E34" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="91" t="s">
+      <c r="G34" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91"/>
+      <c r="H34" s="105"/>
+      <c r="I34" s="105"/>
+      <c r="J34" s="105"/>
       <c r="L34" s="12" t="s">
         <v>4</v>
       </c>
@@ -4789,12 +4789,12 @@
       <c r="O34" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="104" t="s">
+      <c r="Q34" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="R34" s="104"/>
-      <c r="S34" s="104"/>
-      <c r="T34" s="104"/>
+      <c r="R34" s="111"/>
+      <c r="S34" s="111"/>
+      <c r="T34" s="111"/>
     </row>
     <row r="35" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="29" t="s">
@@ -4809,22 +4809,22 @@
       <c r="E35" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="92" t="s">
+      <c r="G35" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="94"/>
-      <c r="L35" s="101" t="s">
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="114"/>
+      <c r="L35" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="M35" s="101" t="s">
+      <c r="M35" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="N35" s="101" t="s">
+      <c r="N35" s="108" t="s">
         <v>89</v>
       </c>
-      <c r="O35" s="101" t="s">
+      <c r="O35" s="108" t="s">
         <v>90</v>
       </c>
       <c r="Q35" s="77" t="s">
@@ -4853,14 +4853,14 @@
       <c r="E36" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="95"/>
-      <c r="H36" s="96"/>
-      <c r="I36" s="96"/>
-      <c r="J36" s="97"/>
-      <c r="L36" s="102"/>
-      <c r="M36" s="102"/>
-      <c r="N36" s="102"/>
-      <c r="O36" s="102"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="116"/>
+      <c r="I36" s="116"/>
+      <c r="J36" s="117"/>
+      <c r="L36" s="109"/>
+      <c r="M36" s="109"/>
+      <c r="N36" s="109"/>
+      <c r="O36" s="109"/>
       <c r="Q36" s="77" t="s">
         <v>92</v>
       </c>
@@ -4890,17 +4890,17 @@
       <c r="F37" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="95"/>
-      <c r="H37" s="96"/>
-      <c r="I37" s="96"/>
-      <c r="J37" s="97"/>
+      <c r="G37" s="115"/>
+      <c r="H37" s="116"/>
+      <c r="I37" s="116"/>
+      <c r="J37" s="117"/>
       <c r="K37" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="102"/>
-      <c r="M37" s="102"/>
-      <c r="N37" s="102"/>
-      <c r="O37" s="102"/>
+      <c r="L37" s="109"/>
+      <c r="M37" s="109"/>
+      <c r="N37" s="109"/>
+      <c r="O37" s="109"/>
       <c r="P37" s="26" t="s">
         <v>60</v>
       </c>
@@ -4930,14 +4930,14 @@
       <c r="E38" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="G38" s="95"/>
-      <c r="H38" s="96"/>
-      <c r="I38" s="96"/>
-      <c r="J38" s="97"/>
-      <c r="L38" s="102"/>
-      <c r="M38" s="102"/>
-      <c r="N38" s="102"/>
-      <c r="O38" s="102"/>
+      <c r="G38" s="115"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="116"/>
+      <c r="J38" s="117"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="109"/>
+      <c r="N38" s="109"/>
+      <c r="O38" s="109"/>
       <c r="Q38" s="77" t="s">
         <v>95</v>
       </c>
@@ -4964,14 +4964,14 @@
       <c r="E39" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="95"/>
-      <c r="H39" s="96"/>
-      <c r="I39" s="96"/>
-      <c r="J39" s="97"/>
-      <c r="L39" s="102"/>
-      <c r="M39" s="102"/>
-      <c r="N39" s="102"/>
-      <c r="O39" s="102"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="116"/>
+      <c r="I39" s="116"/>
+      <c r="J39" s="117"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
+      <c r="N39" s="109"/>
+      <c r="O39" s="109"/>
       <c r="Q39" s="77" t="s">
         <v>96</v>
       </c>
@@ -4998,14 +4998,14 @@
       <c r="E40" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="98"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="99"/>
-      <c r="J40" s="100"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-      <c r="N40" s="103"/>
-      <c r="O40" s="103"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="120"/>
+      <c r="L40" s="110"/>
+      <c r="M40" s="110"/>
+      <c r="N40" s="110"/>
+      <c r="O40" s="110"/>
       <c r="Q40" s="77" t="s">
         <v>97</v>
       </c>
@@ -5023,12 +5023,12 @@
       <c r="C44" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L44" s="89" t="s">
+      <c r="L44" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="M44" s="89"/>
-      <c r="N44" s="89"/>
-      <c r="O44" s="89"/>
+      <c r="M44" s="104"/>
+      <c r="N44" s="104"/>
+      <c r="O44" s="104"/>
     </row>
     <row r="45" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
@@ -5043,12 +5043,12 @@
       <c r="E45" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G45" s="91" t="s">
+      <c r="G45" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H45" s="91"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
+      <c r="H45" s="105"/>
+      <c r="I45" s="105"/>
+      <c r="J45" s="105"/>
       <c r="L45" s="12" t="s">
         <v>4</v>
       </c>
@@ -5061,26 +5061,26 @@
       <c r="O45" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q45" s="91" t="s">
+      <c r="Q45" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="R45" s="91"/>
-      <c r="S45" s="91"/>
-      <c r="T45" s="91"/>
+      <c r="R45" s="105"/>
+      <c r="S45" s="105"/>
+      <c r="T45" s="105"/>
     </row>
     <row r="46" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="50"/>
       <c r="C46" s="50"/>
       <c r="D46" s="50"/>
       <c r="E46" s="50"/>
-      <c r="G46" s="92"/>
-      <c r="H46" s="93"/>
-      <c r="I46" s="93"/>
-      <c r="J46" s="94"/>
-      <c r="L46" s="101"/>
-      <c r="M46" s="101"/>
-      <c r="N46" s="101"/>
-      <c r="O46" s="101"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="113"/>
+      <c r="I46" s="113"/>
+      <c r="J46" s="114"/>
+      <c r="L46" s="108"/>
+      <c r="M46" s="108"/>
+      <c r="N46" s="108"/>
+      <c r="O46" s="108"/>
       <c r="Q46" s="50"/>
       <c r="R46" s="50"/>
       <c r="S46" s="50"/>
@@ -5091,14 +5091,14 @@
       <c r="C47" s="50"/>
       <c r="D47" s="50"/>
       <c r="E47" s="50"/>
-      <c r="G47" s="95"/>
-      <c r="H47" s="96"/>
-      <c r="I47" s="96"/>
-      <c r="J47" s="97"/>
-      <c r="L47" s="102"/>
-      <c r="M47" s="102"/>
-      <c r="N47" s="102"/>
-      <c r="O47" s="102"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="116"/>
+      <c r="I47" s="116"/>
+      <c r="J47" s="117"/>
+      <c r="L47" s="109"/>
+      <c r="M47" s="109"/>
+      <c r="N47" s="109"/>
+      <c r="O47" s="109"/>
       <c r="Q47" s="50"/>
       <c r="R47" s="50"/>
       <c r="S47" s="50"/>
@@ -5112,17 +5112,17 @@
       <c r="F48" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="G48" s="95"/>
-      <c r="H48" s="96"/>
-      <c r="I48" s="96"/>
-      <c r="J48" s="97"/>
+      <c r="G48" s="115"/>
+      <c r="H48" s="116"/>
+      <c r="I48" s="116"/>
+      <c r="J48" s="117"/>
       <c r="K48" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="L48" s="102"/>
-      <c r="M48" s="102"/>
-      <c r="N48" s="102"/>
-      <c r="O48" s="102"/>
+      <c r="L48" s="109"/>
+      <c r="M48" s="109"/>
+      <c r="N48" s="109"/>
+      <c r="O48" s="109"/>
       <c r="P48" s="26" t="s">
         <v>60</v>
       </c>
@@ -5136,14 +5136,14 @@
       <c r="C49" s="50"/>
       <c r="D49" s="50"/>
       <c r="E49" s="50"/>
-      <c r="G49" s="95"/>
-      <c r="H49" s="96"/>
-      <c r="I49" s="96"/>
-      <c r="J49" s="97"/>
-      <c r="L49" s="102"/>
-      <c r="M49" s="102"/>
-      <c r="N49" s="102"/>
-      <c r="O49" s="102"/>
+      <c r="G49" s="115"/>
+      <c r="H49" s="116"/>
+      <c r="I49" s="116"/>
+      <c r="J49" s="117"/>
+      <c r="L49" s="109"/>
+      <c r="M49" s="109"/>
+      <c r="N49" s="109"/>
+      <c r="O49" s="109"/>
       <c r="Q49" s="50"/>
       <c r="R49" s="50"/>
       <c r="S49" s="50"/>
@@ -5154,14 +5154,14 @@
       <c r="C50" s="50"/>
       <c r="D50" s="50"/>
       <c r="E50" s="50"/>
-      <c r="G50" s="95"/>
-      <c r="H50" s="96"/>
-      <c r="I50" s="96"/>
-      <c r="J50" s="97"/>
-      <c r="L50" s="102"/>
-      <c r="M50" s="102"/>
-      <c r="N50" s="102"/>
-      <c r="O50" s="102"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="116"/>
+      <c r="I50" s="116"/>
+      <c r="J50" s="117"/>
+      <c r="L50" s="109"/>
+      <c r="M50" s="109"/>
+      <c r="N50" s="109"/>
+      <c r="O50" s="109"/>
       <c r="Q50" s="50"/>
       <c r="R50" s="50"/>
       <c r="S50" s="50"/>
@@ -5172,53 +5172,53 @@
       <c r="C51" s="50"/>
       <c r="D51" s="50"/>
       <c r="E51" s="50"/>
-      <c r="G51" s="98"/>
-      <c r="H51" s="99"/>
-      <c r="I51" s="99"/>
-      <c r="J51" s="100"/>
-      <c r="L51" s="103"/>
-      <c r="M51" s="103"/>
-      <c r="N51" s="103"/>
-      <c r="O51" s="103"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="119"/>
+      <c r="I51" s="119"/>
+      <c r="J51" s="120"/>
+      <c r="L51" s="110"/>
+      <c r="M51" s="110"/>
+      <c r="N51" s="110"/>
+      <c r="O51" s="110"/>
       <c r="Q51" s="50"/>
       <c r="R51" s="50"/>
       <c r="S51" s="50"/>
       <c r="T51" s="50"/>
     </row>
     <row r="53" spans="1:20" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B53" s="90" t="s">
+      <c r="B53" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90"/>
-      <c r="E53" s="90"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="103"/>
       <c r="F53" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="90" t="s">
+      <c r="G53" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="H53" s="90"/>
-      <c r="I53" s="90"/>
-      <c r="J53" s="90"/>
+      <c r="H53" s="103"/>
+      <c r="I53" s="103"/>
+      <c r="J53" s="103"/>
       <c r="K53" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L53" s="90" t="s">
+      <c r="L53" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="M53" s="90"/>
-      <c r="N53" s="90"/>
-      <c r="O53" s="90"/>
+      <c r="M53" s="103"/>
+      <c r="N53" s="103"/>
+      <c r="O53" s="103"/>
       <c r="P53" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q53" s="90" t="s">
+      <c r="Q53" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="R53" s="90"/>
-      <c r="S53" s="90"/>
-      <c r="T53" s="90"/>
+      <c r="R53" s="103"/>
+      <c r="S53" s="103"/>
+      <c r="T53" s="103"/>
     </row>
     <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="39"/>
@@ -5227,24 +5227,24 @@
       </c>
       <c r="D59" s="39"/>
       <c r="E59" s="39"/>
-      <c r="G59" s="91" t="s">
+      <c r="G59" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H59" s="91"/>
-      <c r="I59" s="91"/>
-      <c r="J59" s="91"/>
-      <c r="L59" s="89" t="s">
+      <c r="H59" s="105"/>
+      <c r="I59" s="105"/>
+      <c r="J59" s="105"/>
+      <c r="L59" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="M59" s="89"/>
-      <c r="N59" s="89"/>
-      <c r="O59" s="89"/>
-      <c r="Q59" s="91" t="s">
+      <c r="M59" s="104"/>
+      <c r="N59" s="104"/>
+      <c r="O59" s="104"/>
+      <c r="Q59" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="R59" s="91"/>
-      <c r="S59" s="91"/>
-      <c r="T59" s="91"/>
+      <c r="R59" s="105"/>
+      <c r="S59" s="105"/>
+      <c r="T59" s="105"/>
     </row>
     <row r="60" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="37"/>
@@ -5253,15 +5253,15 @@
       <c r="D60" s="50"/>
       <c r="E60" s="50"/>
       <c r="F60" s="42"/>
-      <c r="G60" s="105"/>
-      <c r="H60" s="106"/>
-      <c r="I60" s="106"/>
-      <c r="J60" s="106"/>
+      <c r="G60" s="106"/>
+      <c r="H60" s="107"/>
+      <c r="I60" s="107"/>
+      <c r="J60" s="107"/>
       <c r="K60" s="42"/>
-      <c r="L60" s="101"/>
-      <c r="M60" s="101"/>
-      <c r="N60" s="101"/>
-      <c r="O60" s="101"/>
+      <c r="L60" s="108"/>
+      <c r="M60" s="108"/>
+      <c r="N60" s="108"/>
+      <c r="O60" s="108"/>
       <c r="Q60" s="50"/>
       <c r="R60" s="50"/>
       <c r="S60" s="50"/>
@@ -5274,15 +5274,15 @@
       <c r="D61" s="50"/>
       <c r="E61" s="50"/>
       <c r="F61" s="42"/>
-      <c r="G61" s="106"/>
-      <c r="H61" s="106"/>
-      <c r="I61" s="106"/>
-      <c r="J61" s="106"/>
+      <c r="G61" s="107"/>
+      <c r="H61" s="107"/>
+      <c r="I61" s="107"/>
+      <c r="J61" s="107"/>
       <c r="K61" s="42"/>
-      <c r="L61" s="102"/>
-      <c r="M61" s="102"/>
-      <c r="N61" s="102"/>
-      <c r="O61" s="102"/>
+      <c r="L61" s="109"/>
+      <c r="M61" s="109"/>
+      <c r="N61" s="109"/>
+      <c r="O61" s="109"/>
       <c r="Q61" s="50"/>
       <c r="R61" s="50"/>
       <c r="S61" s="50"/>
@@ -5297,17 +5297,17 @@
       <c r="F62" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="G62" s="106"/>
-      <c r="H62" s="106"/>
-      <c r="I62" s="106"/>
-      <c r="J62" s="106"/>
+      <c r="G62" s="107"/>
+      <c r="H62" s="107"/>
+      <c r="I62" s="107"/>
+      <c r="J62" s="107"/>
       <c r="K62" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="L62" s="102"/>
-      <c r="M62" s="102"/>
-      <c r="N62" s="102"/>
-      <c r="O62" s="102"/>
+      <c r="L62" s="109"/>
+      <c r="M62" s="109"/>
+      <c r="N62" s="109"/>
+      <c r="O62" s="109"/>
       <c r="P62" s="26" t="s">
         <v>60</v>
       </c>
@@ -5323,14 +5323,14 @@
       <c r="D63" s="50"/>
       <c r="E63" s="50"/>
       <c r="F63" s="42"/>
-      <c r="G63" s="106"/>
-      <c r="H63" s="106"/>
-      <c r="I63" s="106"/>
-      <c r="J63" s="106"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="102"/>
-      <c r="N63" s="102"/>
-      <c r="O63" s="102"/>
+      <c r="G63" s="107"/>
+      <c r="H63" s="107"/>
+      <c r="I63" s="107"/>
+      <c r="J63" s="107"/>
+      <c r="L63" s="109"/>
+      <c r="M63" s="109"/>
+      <c r="N63" s="109"/>
+      <c r="O63" s="109"/>
       <c r="Q63" s="50"/>
       <c r="R63" s="50"/>
       <c r="S63" s="50"/>
@@ -5343,14 +5343,14 @@
       <c r="D64" s="50"/>
       <c r="E64" s="50"/>
       <c r="F64" s="42"/>
-      <c r="G64" s="106"/>
-      <c r="H64" s="106"/>
-      <c r="I64" s="106"/>
-      <c r="J64" s="106"/>
-      <c r="L64" s="102"/>
-      <c r="M64" s="102"/>
-      <c r="N64" s="102"/>
-      <c r="O64" s="102"/>
+      <c r="G64" s="107"/>
+      <c r="H64" s="107"/>
+      <c r="I64" s="107"/>
+      <c r="J64" s="107"/>
+      <c r="L64" s="109"/>
+      <c r="M64" s="109"/>
+      <c r="N64" s="109"/>
+      <c r="O64" s="109"/>
       <c r="Q64" s="50"/>
       <c r="R64" s="50"/>
       <c r="S64" s="50"/>
@@ -5363,14 +5363,14 @@
       <c r="D65" s="50"/>
       <c r="E65" s="50"/>
       <c r="F65" s="42"/>
-      <c r="G65" s="106"/>
-      <c r="H65" s="106"/>
-      <c r="I65" s="106"/>
-      <c r="J65" s="106"/>
-      <c r="L65" s="103"/>
-      <c r="M65" s="103"/>
-      <c r="N65" s="103"/>
-      <c r="O65" s="103"/>
+      <c r="G65" s="107"/>
+      <c r="H65" s="107"/>
+      <c r="I65" s="107"/>
+      <c r="J65" s="107"/>
+      <c r="L65" s="110"/>
+      <c r="M65" s="110"/>
+      <c r="N65" s="110"/>
+      <c r="O65" s="110"/>
       <c r="Q65" s="50"/>
       <c r="R65" s="50"/>
       <c r="S65" s="50"/>
@@ -5383,66 +5383,42 @@
       <c r="J66" s="56"/>
     </row>
     <row r="67" spans="1:20" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B67" s="90" t="s">
+      <c r="B67" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="90"/>
-      <c r="D67" s="90"/>
-      <c r="E67" s="90"/>
+      <c r="C67" s="103"/>
+      <c r="D67" s="103"/>
+      <c r="E67" s="103"/>
       <c r="F67" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G67" s="90" t="s">
+      <c r="G67" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="H67" s="90"/>
-      <c r="I67" s="90"/>
-      <c r="J67" s="90"/>
+      <c r="H67" s="103"/>
+      <c r="I67" s="103"/>
+      <c r="J67" s="103"/>
       <c r="K67" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L67" s="90" t="s">
+      <c r="L67" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="M67" s="90"/>
-      <c r="N67" s="90"/>
-      <c r="O67" s="90"/>
+      <c r="M67" s="103"/>
+      <c r="N67" s="103"/>
+      <c r="O67" s="103"/>
       <c r="P67" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q67" s="90" t="s">
+      <c r="Q67" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="R67" s="90"/>
-      <c r="S67" s="90"/>
-      <c r="T67" s="90"/>
+      <c r="R67" s="103"/>
+      <c r="S67" s="103"/>
+      <c r="T67" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="G67:J67"/>
-    <mergeCell ref="L67:O67"/>
-    <mergeCell ref="Q67:T67"/>
-    <mergeCell ref="L59:O59"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="Q59:T59"/>
-    <mergeCell ref="G60:J65"/>
-    <mergeCell ref="L60:L65"/>
-    <mergeCell ref="M60:M65"/>
-    <mergeCell ref="N60:N65"/>
-    <mergeCell ref="O60:O65"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="Q34:T34"/>
-    <mergeCell ref="G35:J40"/>
-    <mergeCell ref="L35:L40"/>
-    <mergeCell ref="M35:M40"/>
-    <mergeCell ref="N35:N40"/>
-    <mergeCell ref="O35:O40"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="Q12:T12"/>
-    <mergeCell ref="L33:O33"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="G53:J53"/>
@@ -5459,6 +5435,30 @@
     <mergeCell ref="O46:O51"/>
     <mergeCell ref="L23:O23"/>
     <mergeCell ref="G24:J24"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="Q34:T34"/>
+    <mergeCell ref="G35:J40"/>
+    <mergeCell ref="L35:L40"/>
+    <mergeCell ref="M35:M40"/>
+    <mergeCell ref="N35:N40"/>
+    <mergeCell ref="O35:O40"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="L67:O67"/>
+    <mergeCell ref="Q67:T67"/>
+    <mergeCell ref="L59:O59"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="Q59:T59"/>
+    <mergeCell ref="G60:J65"/>
+    <mergeCell ref="L60:L65"/>
+    <mergeCell ref="M60:M65"/>
+    <mergeCell ref="N60:N65"/>
+    <mergeCell ref="O60:O65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6004,7 +6004,7 @@
       <c r="S7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="108" t="s">
+      <c r="U7" s="121" t="s">
         <v>37</v>
       </c>
       <c r="V7" s="8" t="s">
@@ -6016,7 +6016,7 @@
       <c r="X7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" s="108" t="s">
+      <c r="Z7" s="121" t="s">
         <v>37</v>
       </c>
       <c r="AA7" s="8" t="s">
@@ -6048,7 +6048,7 @@
       <c r="S8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="108"/>
+      <c r="U8" s="121"/>
       <c r="V8" s="14" t="s">
         <v>26</v>
       </c>
@@ -6058,7 +6058,7 @@
       <c r="X8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" s="108"/>
+      <c r="Z8" s="121"/>
       <c r="AA8" s="14" t="s">
         <v>26</v>
       </c>
@@ -6088,7 +6088,7 @@
       <c r="S9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="U9" s="109" t="s">
+      <c r="U9" s="122" t="s">
         <v>38</v>
       </c>
       <c r="V9" s="11" t="s">
@@ -6100,7 +6100,7 @@
       <c r="X9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Z9" s="109" t="s">
+      <c r="Z9" s="122" t="s">
         <v>38</v>
       </c>
       <c r="AA9" s="11" t="s">
@@ -6123,7 +6123,7 @@
       <c r="S10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="U10" s="109"/>
+      <c r="U10" s="122"/>
       <c r="V10" s="14" t="s">
         <v>28</v>
       </c>
@@ -6133,7 +6133,7 @@
       <c r="X10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Z10" s="109"/>
+      <c r="Z10" s="122"/>
       <c r="AA10" s="14" t="s">
         <v>28</v>
       </c>
@@ -6223,24 +6223,24 @@
       </c>
     </row>
     <row r="26" spans="7:43" x14ac:dyDescent="0.25">
-      <c r="AB26" s="107" t="s">
+      <c r="AB26" s="123" t="s">
         <v>118</v>
       </c>
-      <c r="AC26" s="107"/>
-      <c r="AD26" s="107"/>
-      <c r="AE26" s="107"/>
-      <c r="AH26" s="107" t="s">
+      <c r="AC26" s="123"/>
+      <c r="AD26" s="123"/>
+      <c r="AE26" s="123"/>
+      <c r="AH26" s="123" t="s">
         <v>50</v>
       </c>
-      <c r="AI26" s="107"/>
-      <c r="AJ26" s="107"/>
-      <c r="AK26" s="107"/>
-      <c r="AN26" s="107" t="s">
+      <c r="AI26" s="123"/>
+      <c r="AJ26" s="123"/>
+      <c r="AK26" s="123"/>
+      <c r="AN26" s="123" t="s">
         <v>119</v>
       </c>
-      <c r="AO26" s="107"/>
-      <c r="AP26" s="107"/>
-      <c r="AQ26" s="107"/>
+      <c r="AO26" s="123"/>
+      <c r="AP26" s="123"/>
+      <c r="AQ26" s="123"/>
     </row>
     <row r="27" spans="7:43" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
@@ -6369,7 +6369,7 @@
       <c r="AE28" s="10">
         <v>24.39</v>
       </c>
-      <c r="AG28" s="108" t="s">
+      <c r="AG28" s="121" t="s">
         <v>117</v>
       </c>
       <c r="AH28" s="8">
@@ -6384,7 +6384,7 @@
       <c r="AK28" s="10">
         <v>24.39</v>
       </c>
-      <c r="AM28" s="108" t="s">
+      <c r="AM28" s="121" t="s">
         <v>117</v>
       </c>
       <c r="AN28" s="8">
@@ -6455,7 +6455,7 @@
       <c r="AE29" s="13">
         <v>21.45</v>
       </c>
-      <c r="AG29" s="108"/>
+      <c r="AG29" s="121"/>
       <c r="AH29" s="11">
         <v>24.21</v>
       </c>
@@ -6468,7 +6468,7 @@
       <c r="AK29" s="13">
         <v>21.45</v>
       </c>
-      <c r="AM29" s="108"/>
+      <c r="AM29" s="121"/>
       <c r="AN29" s="11">
         <v>24.21</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="AE30" s="13">
         <v>32.74</v>
       </c>
-      <c r="AG30" s="108"/>
+      <c r="AG30" s="121"/>
       <c r="AH30" s="11">
         <v>26.88</v>
       </c>
@@ -6550,7 +6550,7 @@
       <c r="AK30" s="13">
         <v>32.74</v>
       </c>
-      <c r="AM30" s="108"/>
+      <c r="AM30" s="121"/>
       <c r="AN30" s="14">
         <v>26.88</v>
       </c>
@@ -6598,7 +6598,7 @@
       <c r="AE31" s="13">
         <v>24.21</v>
       </c>
-      <c r="AG31" s="108" t="s">
+      <c r="AG31" s="121" t="s">
         <v>116</v>
       </c>
       <c r="AH31" s="8">
@@ -6613,7 +6613,7 @@
       <c r="AK31" s="10">
         <v>24.21</v>
       </c>
-      <c r="AM31" s="108" t="s">
+      <c r="AM31" s="121" t="s">
         <v>116</v>
       </c>
       <c r="AN31" s="11">
@@ -6663,7 +6663,7 @@
       <c r="AE32" s="13">
         <v>25.67</v>
       </c>
-      <c r="AG32" s="108"/>
+      <c r="AG32" s="121"/>
       <c r="AH32" s="11">
         <v>23.4</v>
       </c>
@@ -6676,7 +6676,7 @@
       <c r="AK32" s="13">
         <v>25.67</v>
       </c>
-      <c r="AM32" s="108"/>
+      <c r="AM32" s="121"/>
       <c r="AN32" s="11">
         <v>23.4</v>
       </c>
@@ -6724,7 +6724,7 @@
       <c r="AE33" s="16">
         <v>23.42</v>
       </c>
-      <c r="AG33" s="108"/>
+      <c r="AG33" s="121"/>
       <c r="AH33" s="14">
         <v>23.35</v>
       </c>
@@ -6737,7 +6737,7 @@
       <c r="AK33" s="16">
         <v>23.42</v>
       </c>
-      <c r="AM33" s="108"/>
+      <c r="AM33" s="121"/>
       <c r="AN33" s="14">
         <v>23.35</v>
       </c>
@@ -6858,7 +6858,7 @@
       <c r="AE37" s="10">
         <v>24.39</v>
       </c>
-      <c r="AG37" s="108" t="s">
+      <c r="AG37" s="121" t="s">
         <v>42</v>
       </c>
       <c r="AH37" s="8">
@@ -6873,7 +6873,7 @@
       <c r="AK37" s="10">
         <v>24.39</v>
       </c>
-      <c r="AM37" s="109" t="s">
+      <c r="AM37" s="122" t="s">
         <v>42</v>
       </c>
       <c r="AN37" s="8">
@@ -6911,7 +6911,7 @@
       <c r="AE38" s="13">
         <v>21.45</v>
       </c>
-      <c r="AG38" s="108"/>
+      <c r="AG38" s="121"/>
       <c r="AH38" s="11">
         <v>24.21</v>
       </c>
@@ -6924,7 +6924,7 @@
       <c r="AK38" s="13">
         <v>21.45</v>
       </c>
-      <c r="AM38" s="109"/>
+      <c r="AM38" s="122"/>
       <c r="AN38" s="11">
         <v>24.21</v>
       </c>
@@ -6960,7 +6960,7 @@
       <c r="AE39" s="13">
         <v>32.74</v>
       </c>
-      <c r="AG39" s="108"/>
+      <c r="AG39" s="121"/>
       <c r="AH39" s="11">
         <v>26.88</v>
       </c>
@@ -6973,7 +6973,7 @@
       <c r="AK39" s="13">
         <v>32.74</v>
       </c>
-      <c r="AM39" s="109"/>
+      <c r="AM39" s="122"/>
       <c r="AN39" s="14">
         <v>26.88</v>
       </c>
@@ -7009,7 +7009,7 @@
       <c r="AE40" s="13">
         <v>24.21</v>
       </c>
-      <c r="AG40" s="108" t="s">
+      <c r="AG40" s="121" t="s">
         <v>43</v>
       </c>
       <c r="AH40" s="8">
@@ -7024,7 +7024,7 @@
       <c r="AK40" s="10">
         <v>24.21</v>
       </c>
-      <c r="AM40" s="109" t="s">
+      <c r="AM40" s="122" t="s">
         <v>43</v>
       </c>
       <c r="AN40" s="11">
@@ -7062,7 +7062,7 @@
       <c r="AE41" s="13">
         <v>25.67</v>
       </c>
-      <c r="AG41" s="108"/>
+      <c r="AG41" s="121"/>
       <c r="AH41" s="11">
         <v>23.4</v>
       </c>
@@ -7075,7 +7075,7 @@
       <c r="AK41" s="13">
         <v>25.67</v>
       </c>
-      <c r="AM41" s="109"/>
+      <c r="AM41" s="122"/>
       <c r="AN41" s="11">
         <v>23.4</v>
       </c>
@@ -7111,7 +7111,7 @@
       <c r="AE42" s="16">
         <v>23.42</v>
       </c>
-      <c r="AG42" s="108"/>
+      <c r="AG42" s="121"/>
       <c r="AH42" s="14">
         <v>23.35</v>
       </c>
@@ -7124,7 +7124,7 @@
       <c r="AK42" s="16">
         <v>23.42</v>
       </c>
-      <c r="AM42" s="109"/>
+      <c r="AM42" s="122"/>
       <c r="AN42" s="14">
         <v>23.35</v>
       </c>
@@ -7626,6 +7626,11 @@
     <sortCondition ref="H27:H51"/>
   </sortState>
   <mergeCells count="15">
+    <mergeCell ref="AN26:AQ26"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="AG40:AG42"/>
     <mergeCell ref="AM40:AM42"/>
     <mergeCell ref="AG31:AG33"/>
@@ -7636,11 +7641,6 @@
     <mergeCell ref="AG37:AG39"/>
     <mergeCell ref="AM37:AM39"/>
     <mergeCell ref="AH26:AK26"/>
-    <mergeCell ref="AN26:AQ26"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="Z9:Z10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7651,7 +7651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:AL38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -7678,36 +7678,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="G2" s="110" t="s">
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="G2" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="L2" s="110" t="s">
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="L2" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="Q2" s="112" t="s">
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="Q2" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="V2" s="91" t="s">
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="V2" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="91"/>
-      <c r="X2" s="91"/>
-      <c r="Y2" s="91"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
@@ -7866,26 +7866,26 @@
       <c r="Y8" s="46"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="L10" s="91" t="s">
+      <c r="L10" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="91"/>
+      <c r="M10" s="105"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="105"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
-      <c r="G11" s="110" t="s">
+      <c r="C11" s="111"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="G11" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
       <c r="L11" s="12" t="s">
         <v>154</v>
       </c>
@@ -7898,24 +7898,24 @@
       <c r="O11" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="Q11" s="110" t="s">
+      <c r="Q11" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="110"/>
-      <c r="S11" s="110"/>
-      <c r="T11" s="110"/>
-      <c r="V11" s="112" t="s">
+      <c r="R11" s="124"/>
+      <c r="S11" s="124"/>
+      <c r="T11" s="124"/>
+      <c r="V11" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="W11" s="110"/>
-      <c r="X11" s="110"/>
-      <c r="Y11" s="110"/>
-      <c r="AA11" s="110" t="s">
+      <c r="W11" s="124"/>
+      <c r="X11" s="124"/>
+      <c r="Y11" s="124"/>
+      <c r="AA11" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AB11" s="110"/>
-      <c r="AC11" s="110"/>
-      <c r="AD11" s="110"/>
+      <c r="AB11" s="124"/>
+      <c r="AC11" s="124"/>
+      <c r="AD11" s="124"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="46">
@@ -8494,26 +8494,26 @@
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="L21" s="91" t="s">
+      <c r="L21" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="M21" s="91"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="91"/>
+      <c r="M21" s="105"/>
+      <c r="N21" s="105"/>
+      <c r="O21" s="105"/>
     </row>
     <row r="22" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="G22" s="110" t="s">
+      <c r="C22" s="111"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="G22" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
+      <c r="H22" s="124"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
       <c r="L22" s="12" t="s">
         <v>154</v>
       </c>
@@ -8526,24 +8526,24 @@
       <c r="O22" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="Q22" s="110" t="s">
+      <c r="Q22" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="R22" s="110"/>
-      <c r="S22" s="110"/>
-      <c r="T22" s="110"/>
-      <c r="V22" s="112" t="s">
+      <c r="R22" s="124"/>
+      <c r="S22" s="124"/>
+      <c r="T22" s="124"/>
+      <c r="V22" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="W22" s="110"/>
-      <c r="X22" s="110"/>
-      <c r="Y22" s="110"/>
-      <c r="AA22" s="110" t="s">
+      <c r="W22" s="124"/>
+      <c r="X22" s="124"/>
+      <c r="Y22" s="124"/>
+      <c r="AA22" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AB22" s="110"/>
-      <c r="AC22" s="110"/>
-      <c r="AD22" s="110"/>
+      <c r="AB22" s="124"/>
+      <c r="AC22" s="124"/>
+      <c r="AD22" s="124"/>
     </row>
     <row r="23" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="46">
@@ -9143,26 +9143,26 @@
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="L31" s="91" t="s">
+      <c r="L31" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="M31" s="91"/>
-      <c r="N31" s="91"/>
-      <c r="O31" s="91"/>
+      <c r="M31" s="105"/>
+      <c r="N31" s="105"/>
+      <c r="O31" s="105"/>
     </row>
     <row r="32" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="91" t="s">
+      <c r="B32" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="104"/>
-      <c r="G32" s="91" t="s">
+      <c r="C32" s="111"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="111"/>
+      <c r="G32" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H32" s="91"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="105"/>
+      <c r="J32" s="105"/>
       <c r="L32" s="12" t="s">
         <v>154</v>
       </c>
@@ -9175,24 +9175,24 @@
       <c r="O32" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="Q32" s="91" t="s">
+      <c r="Q32" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="R32" s="91"/>
-      <c r="S32" s="91"/>
-      <c r="T32" s="91"/>
-      <c r="V32" s="111" t="s">
+      <c r="R32" s="105"/>
+      <c r="S32" s="105"/>
+      <c r="T32" s="105"/>
+      <c r="V32" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="W32" s="91"/>
-      <c r="X32" s="91"/>
-      <c r="Y32" s="91"/>
-      <c r="AA32" s="110" t="s">
+      <c r="W32" s="105"/>
+      <c r="X32" s="105"/>
+      <c r="Y32" s="105"/>
+      <c r="AA32" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AB32" s="110"/>
-      <c r="AC32" s="110"/>
-      <c r="AD32" s="110"/>
+      <c r="AB32" s="124"/>
+      <c r="AC32" s="124"/>
+      <c r="AD32" s="124"/>
       <c r="AH32" s="1" t="s">
         <v>126</v>
       </c>
@@ -9909,14 +9909,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="V11:Y11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA32:AD32"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="Q32:T32"/>
+    <mergeCell ref="V32:Y32"/>
     <mergeCell ref="AA11:AD11"/>
     <mergeCell ref="L21:O21"/>
     <mergeCell ref="B22:E22"/>
@@ -9926,12 +9924,14 @@
     <mergeCell ref="AA22:AD22"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="G11:J11"/>
-    <mergeCell ref="AA32:AD32"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="Q32:T32"/>
-    <mergeCell ref="V32:Y32"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="V11:Y11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9942,49 +9942,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5260BD5D-0539-41D9-9873-5C11F72F59A0}">
   <dimension ref="A2:Y52"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="5" width="7.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="1" customWidth="1"/>
+    <col min="7" max="10" width="7.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="1" customWidth="1"/>
+    <col min="12" max="15" width="7.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="20" width="7.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" style="1" customWidth="1"/>
+    <col min="22" max="25" width="7.28515625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="39"/>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="92" t="s">
         <v>58</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
-      <c r="G2" s="91" t="s">
+      <c r="G2" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="L2" s="115" t="s">
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="L2" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="Q2" s="91" t="s">
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="Q2" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="91"/>
-      <c r="V2" s="91" t="s">
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="V2" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="91"/>
-      <c r="X2" s="91"/>
-      <c r="Y2" s="91"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
     </row>
     <row r="3" spans="2:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="50"/>
@@ -9992,19 +9999,19 @@
       <c r="D3" s="50"/>
       <c r="E3" s="50"/>
       <c r="F3" s="42"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
       <c r="K3" s="42"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="118"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="90"/>
+      <c r="S3" s="90"/>
+      <c r="T3" s="91"/>
       <c r="V3" s="50"/>
       <c r="W3" s="50"/>
       <c r="X3" s="50"/>
@@ -10016,19 +10023,19 @@
       <c r="D4" s="50"/>
       <c r="E4" s="50"/>
       <c r="F4" s="42"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
       <c r="K4" s="42"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="118"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="91"/>
       <c r="V4" s="50"/>
       <c r="W4" s="50"/>
       <c r="X4" s="50"/>
@@ -10042,24 +10049,24 @@
       <c r="F5" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
       <c r="K5" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102"/>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
       <c r="P5" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="118"/>
+      <c r="Q5" s="89"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="90"/>
+      <c r="T5" s="91"/>
       <c r="U5" s="26" t="s">
         <v>60</v>
       </c>
@@ -10074,18 +10081,18 @@
       <c r="D6" s="50"/>
       <c r="E6" s="50"/>
       <c r="F6" s="42"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="102"/>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="118"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="91"/>
       <c r="V6" s="50"/>
       <c r="W6" s="50"/>
       <c r="X6" s="50"/>
@@ -10097,18 +10104,18 @@
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
       <c r="F7" s="42"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="102"/>
-      <c r="N7" s="102"/>
-      <c r="O7" s="102"/>
-      <c r="Q7" s="116"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="118"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="90"/>
+      <c r="T7" s="91"/>
       <c r="V7" s="50"/>
       <c r="W7" s="50"/>
       <c r="X7" s="50"/>
@@ -10120,18 +10127,18 @@
       <c r="D8" s="50"/>
       <c r="E8" s="50"/>
       <c r="F8" s="42"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="118"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
       <c r="V8" s="50"/>
       <c r="W8" s="50"/>
       <c r="X8" s="50"/>
@@ -10144,78 +10151,78 @@
       <c r="J9" s="56"/>
     </row>
     <row r="10" spans="2:25" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
       <c r="F10" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="90" t="s">
+      <c r="G10" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="103"/>
       <c r="K10" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="90" t="s">
+      <c r="L10" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="90"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="103"/>
+      <c r="O10" s="103"/>
       <c r="P10" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="90" t="s">
+      <c r="Q10" s="103" t="s">
         <v>163</v>
       </c>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
+      <c r="R10" s="103"/>
+      <c r="S10" s="103"/>
+      <c r="T10" s="103"/>
       <c r="U10" s="51"/>
-      <c r="V10" s="90" t="s">
+      <c r="V10" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="W10" s="90"/>
-      <c r="X10" s="90"/>
-      <c r="Y10" s="90"/>
+      <c r="W10" s="103"/>
+      <c r="X10" s="103"/>
+      <c r="Y10" s="103"/>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="39"/>
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="92" t="s">
         <v>58</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
-      <c r="G13" s="91" t="s">
+      <c r="G13" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="L13" s="115" t="s">
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="L13" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="M13" s="115"/>
-      <c r="N13" s="115"/>
-      <c r="O13" s="115"/>
-      <c r="Q13" s="91" t="s">
+      <c r="M13" s="105"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="105"/>
+      <c r="Q13" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="R13" s="91"/>
-      <c r="S13" s="91"/>
-      <c r="T13" s="91"/>
-      <c r="V13" s="91" t="s">
+      <c r="R13" s="105"/>
+      <c r="S13" s="105"/>
+      <c r="T13" s="105"/>
+      <c r="V13" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="W13" s="91"/>
-      <c r="X13" s="91"/>
-      <c r="Y13" s="91"/>
+      <c r="W13" s="105"/>
+      <c r="X13" s="105"/>
+      <c r="Y13" s="105"/>
     </row>
     <row r="14" spans="2:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="50"/>
@@ -10223,19 +10230,19 @@
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
       <c r="F14" s="42"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106"/>
-      <c r="J14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
       <c r="K14" s="42"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
-      <c r="Q14" s="116"/>
-      <c r="R14" s="117"/>
-      <c r="S14" s="117"/>
-      <c r="T14" s="118"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="91"/>
       <c r="V14" s="50"/>
       <c r="W14" s="50"/>
       <c r="X14" s="50"/>
@@ -10247,19 +10254,19 @@
       <c r="D15" s="50"/>
       <c r="E15" s="50"/>
       <c r="F15" s="42"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107"/>
+      <c r="J15" s="107"/>
       <c r="K15" s="42"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="102"/>
-      <c r="O15" s="102"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="117"/>
-      <c r="S15" s="117"/>
-      <c r="T15" s="118"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="109"/>
+      <c r="N15" s="109"/>
+      <c r="O15" s="109"/>
+      <c r="Q15" s="89"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="90"/>
+      <c r="T15" s="91"/>
       <c r="V15" s="50"/>
       <c r="W15" s="50"/>
       <c r="X15" s="50"/>
@@ -10273,20 +10280,20 @@
       <c r="F16" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="106"/>
-      <c r="J16" s="106"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
       <c r="K16" s="70"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="109"/>
+      <c r="N16" s="109"/>
+      <c r="O16" s="109"/>
       <c r="P16" s="26"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="117"/>
-      <c r="S16" s="117"/>
-      <c r="T16" s="118"/>
+      <c r="Q16" s="89"/>
+      <c r="R16" s="90"/>
+      <c r="S16" s="90"/>
+      <c r="T16" s="91"/>
       <c r="U16" s="26"/>
       <c r="V16" s="50"/>
       <c r="W16" s="50"/>
@@ -10299,18 +10306,18 @@
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
       <c r="F17" s="42"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-      <c r="Q17" s="116"/>
-      <c r="R17" s="117"/>
-      <c r="S17" s="117"/>
-      <c r="T17" s="118"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="L17" s="109"/>
+      <c r="M17" s="109"/>
+      <c r="N17" s="109"/>
+      <c r="O17" s="109"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="91"/>
       <c r="V17" s="50"/>
       <c r="W17" s="50"/>
       <c r="X17" s="50"/>
@@ -10322,18 +10329,18 @@
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
       <c r="F18" s="42"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="102"/>
-      <c r="O18" s="102"/>
-      <c r="Q18" s="116"/>
-      <c r="R18" s="117"/>
-      <c r="S18" s="117"/>
-      <c r="T18" s="118"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="107"/>
+      <c r="J18" s="107"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="109"/>
+      <c r="O18" s="109"/>
+      <c r="Q18" s="89"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="91"/>
       <c r="V18" s="50"/>
       <c r="W18" s="50"/>
       <c r="X18" s="50"/>
@@ -10345,18 +10352,18 @@
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
       <c r="F19" s="42"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="106"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
-      <c r="N19" s="103"/>
-      <c r="O19" s="103"/>
-      <c r="Q19" s="116"/>
-      <c r="R19" s="117"/>
-      <c r="S19" s="117"/>
-      <c r="T19" s="118"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="107"/>
+      <c r="J19" s="107"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="110"/>
+      <c r="N19" s="110"/>
+      <c r="O19" s="110"/>
+      <c r="Q19" s="89"/>
+      <c r="R19" s="90"/>
+      <c r="S19" s="90"/>
+      <c r="T19" s="91"/>
       <c r="V19" s="50"/>
       <c r="W19" s="50"/>
       <c r="X19" s="50"/>
@@ -10368,26 +10375,26 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L23" s="91" t="s">
+      <c r="L23" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="M23" s="91"/>
-      <c r="N23" s="91"/>
-      <c r="O23" s="91"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="G24" s="110" t="s">
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="G24" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="110"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="110"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="124"/>
       <c r="L24" s="12" t="s">
         <v>154</v>
       </c>
@@ -10400,18 +10407,18 @@
       <c r="O24" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="Q24" s="110" t="s">
+      <c r="Q24" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="R24" s="110"/>
-      <c r="S24" s="110"/>
-      <c r="T24" s="110"/>
-      <c r="V24" s="110" t="s">
+      <c r="R24" s="124"/>
+      <c r="S24" s="124"/>
+      <c r="T24" s="124"/>
+      <c r="V24" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="W24" s="110"/>
-      <c r="X24" s="110"/>
-      <c r="Y24" s="110"/>
+      <c r="W24" s="124"/>
+      <c r="X24" s="124"/>
+      <c r="Y24" s="124"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="46">
@@ -10455,19 +10462,19 @@
         <v>25.313333333333343</v>
       </c>
       <c r="P25" s="42"/>
-      <c r="Q25" s="120">
+      <c r="Q25" s="93">
         <f>AVERAGE($B$25:$E$25)</f>
         <v>21.912500000000001</v>
       </c>
-      <c r="R25" s="121">
+      <c r="R25" s="94">
         <f t="shared" ref="R25:T25" si="1">AVERAGE($B$25:$E$25)</f>
         <v>21.912500000000001</v>
       </c>
-      <c r="S25" s="121">
+      <c r="S25" s="94">
         <f t="shared" si="1"/>
         <v>21.912500000000001</v>
       </c>
-      <c r="T25" s="122">
+      <c r="T25" s="95">
         <f t="shared" si="1"/>
         <v>21.912500000000001</v>
       </c>
@@ -10531,19 +10538,19 @@
         <v>25.313333333333343</v>
       </c>
       <c r="P26" s="42"/>
-      <c r="Q26" s="120">
+      <c r="Q26" s="93">
         <f>AVERAGE($B$26:$E$26)</f>
         <v>22.2425</v>
       </c>
-      <c r="R26" s="121">
+      <c r="R26" s="94">
         <f t="shared" ref="R26:T26" si="4">AVERAGE($B$26:$E$26)</f>
         <v>22.2425</v>
       </c>
-      <c r="S26" s="121">
+      <c r="S26" s="94">
         <f t="shared" si="4"/>
         <v>22.2425</v>
       </c>
-      <c r="T26" s="122">
+      <c r="T26" s="95">
         <f t="shared" si="4"/>
         <v>22.2425</v>
       </c>
@@ -10607,19 +10614,19 @@
         <v>25.313333333333343</v>
       </c>
       <c r="P27" s="42"/>
-      <c r="Q27" s="120">
+      <c r="Q27" s="93">
         <f>AVERAGE($B$27:$E$27)</f>
         <v>24.619999999999997</v>
       </c>
-      <c r="R27" s="121">
+      <c r="R27" s="94">
         <f t="shared" ref="R27:T27" si="6">AVERAGE($B$27:$E$27)</f>
         <v>24.619999999999997</v>
       </c>
-      <c r="S27" s="121">
+      <c r="S27" s="94">
         <f t="shared" si="6"/>
         <v>24.619999999999997</v>
       </c>
-      <c r="T27" s="122">
+      <c r="T27" s="95">
         <f t="shared" si="6"/>
         <v>24.619999999999997</v>
       </c>
@@ -10683,19 +10690,19 @@
         <v>25.313333333333343</v>
       </c>
       <c r="P28" s="42"/>
-      <c r="Q28" s="120">
+      <c r="Q28" s="93">
         <f>AVERAGE($B$28:$E$28)</f>
         <v>22.747500000000002</v>
       </c>
-      <c r="R28" s="121">
+      <c r="R28" s="94">
         <f t="shared" ref="R28:T28" si="7">AVERAGE($B$28:$E$28)</f>
         <v>22.747500000000002</v>
       </c>
-      <c r="S28" s="121">
+      <c r="S28" s="94">
         <f t="shared" si="7"/>
         <v>22.747500000000002</v>
       </c>
-      <c r="T28" s="122">
+      <c r="T28" s="95">
         <f t="shared" si="7"/>
         <v>22.747500000000002</v>
       </c>
@@ -10759,19 +10766,19 @@
         <v>25.313333333333343</v>
       </c>
       <c r="P29" s="42"/>
-      <c r="Q29" s="120">
+      <c r="Q29" s="93">
         <f>AVERAGE($B$29:$E$29)</f>
         <v>22.625</v>
       </c>
-      <c r="R29" s="121">
+      <c r="R29" s="94">
         <f t="shared" ref="R29:T29" si="8">AVERAGE($B$29:$E$29)</f>
         <v>22.625</v>
       </c>
-      <c r="S29" s="121">
+      <c r="S29" s="94">
         <f t="shared" si="8"/>
         <v>22.625</v>
       </c>
-      <c r="T29" s="122">
+      <c r="T29" s="95">
         <f t="shared" si="8"/>
         <v>22.625</v>
       </c>
@@ -10835,19 +10842,19 @@
         <v>25.313333333333343</v>
       </c>
       <c r="P30" s="42"/>
-      <c r="Q30" s="120">
+      <c r="Q30" s="93">
         <f>AVERAGE($B$30:$E$30)</f>
         <v>22.44</v>
       </c>
-      <c r="R30" s="121">
+      <c r="R30" s="94">
         <f t="shared" ref="R30:T30" si="9">AVERAGE($B$30:$E$30)</f>
         <v>22.44</v>
       </c>
-      <c r="S30" s="121">
+      <c r="S30" s="94">
         <f t="shared" si="9"/>
         <v>22.44</v>
       </c>
-      <c r="T30" s="122">
+      <c r="T30" s="95">
         <f t="shared" si="9"/>
         <v>22.44</v>
       </c>
@@ -10875,26 +10882,26 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L33" s="91" t="s">
+      <c r="L33" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="M33" s="91"/>
-      <c r="N33" s="91"/>
-      <c r="O33" s="91"/>
+      <c r="M33" s="105"/>
+      <c r="N33" s="105"/>
+      <c r="O33" s="105"/>
     </row>
     <row r="34" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="G34" s="110" t="s">
+      <c r="C34" s="111"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="111"/>
+      <c r="G34" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H34" s="110"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
+      <c r="H34" s="124"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="124"/>
       <c r="L34" s="12" t="s">
         <v>154</v>
       </c>
@@ -10907,18 +10914,18 @@
       <c r="O34" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="Q34" s="110" t="s">
+      <c r="Q34" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="R34" s="110"/>
-      <c r="S34" s="110"/>
-      <c r="T34" s="110"/>
-      <c r="V34" s="110" t="s">
+      <c r="R34" s="124"/>
+      <c r="S34" s="124"/>
+      <c r="T34" s="124"/>
+      <c r="V34" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="W34" s="110"/>
-      <c r="X34" s="110"/>
-      <c r="Y34" s="110"/>
+      <c r="W34" s="124"/>
+      <c r="X34" s="124"/>
+      <c r="Y34" s="124"/>
     </row>
     <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="46">
@@ -10966,19 +10973,19 @@
         <v>2.5487500000000125</v>
       </c>
       <c r="P35" s="42"/>
-      <c r="Q35" s="120">
+      <c r="Q35" s="93">
         <f>Q25-G35</f>
         <v>-0.85208333333332931</v>
       </c>
-      <c r="R35" s="121">
+      <c r="R35" s="94">
         <f t="shared" ref="R35:T35" si="12">R25-H35</f>
         <v>-0.85208333333332931</v>
       </c>
-      <c r="S35" s="121">
+      <c r="S35" s="94">
         <f t="shared" si="12"/>
         <v>-0.85208333333332931</v>
       </c>
-      <c r="T35" s="122">
+      <c r="T35" s="95">
         <f t="shared" si="12"/>
         <v>-0.85208333333332931</v>
       </c>
@@ -11046,19 +11053,19 @@
         <v>2.5487500000000125</v>
       </c>
       <c r="P36" s="42"/>
-      <c r="Q36" s="120">
+      <c r="Q36" s="93">
         <f t="shared" ref="Q36:T36" si="16">Q26-G36</f>
         <v>-0.52208333333333101</v>
       </c>
-      <c r="R36" s="121">
+      <c r="R36" s="94">
         <f t="shared" si="16"/>
         <v>-0.52208333333333101</v>
       </c>
-      <c r="S36" s="121">
+      <c r="S36" s="94">
         <f t="shared" si="16"/>
         <v>-0.52208333333333101</v>
       </c>
-      <c r="T36" s="122">
+      <c r="T36" s="95">
         <f t="shared" si="16"/>
         <v>-0.52208333333333101</v>
       </c>
@@ -11134,19 +11141,19 @@
       <c r="P37" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="Q37" s="120">
+      <c r="Q37" s="93">
         <f t="shared" ref="Q37:T37" si="19">Q27-G37</f>
         <v>1.8554166666666667</v>
       </c>
-      <c r="R37" s="121">
+      <c r="R37" s="94">
         <f t="shared" si="19"/>
         <v>1.8554166666666667</v>
       </c>
-      <c r="S37" s="121">
+      <c r="S37" s="94">
         <f t="shared" si="19"/>
         <v>1.8554166666666667</v>
       </c>
-      <c r="T37" s="122">
+      <c r="T37" s="95">
         <f t="shared" si="19"/>
         <v>1.8554166666666667</v>
       </c>
@@ -11216,19 +11223,19 @@
         <v>2.5487500000000125</v>
       </c>
       <c r="P38" s="42"/>
-      <c r="Q38" s="120">
+      <c r="Q38" s="93">
         <f t="shared" ref="Q38:T38" si="22">Q28-G38</f>
         <v>-1.7083333333328454E-2</v>
       </c>
-      <c r="R38" s="121">
+      <c r="R38" s="94">
         <f t="shared" si="22"/>
         <v>-1.7083333333328454E-2</v>
       </c>
-      <c r="S38" s="121">
+      <c r="S38" s="94">
         <f t="shared" si="22"/>
         <v>-1.7083333333328454E-2</v>
       </c>
-      <c r="T38" s="122">
+      <c r="T38" s="95">
         <f t="shared" si="22"/>
         <v>-1.7083333333328454E-2</v>
       </c>
@@ -11296,19 +11303,19 @@
         <v>2.5487500000000125</v>
       </c>
       <c r="P39" s="42"/>
-      <c r="Q39" s="120">
+      <c r="Q39" s="93">
         <f t="shared" ref="Q39:T39" si="25">Q29-G39</f>
         <v>-0.13958333333333073</v>
       </c>
-      <c r="R39" s="121">
+      <c r="R39" s="94">
         <f t="shared" si="25"/>
         <v>-0.13958333333333073</v>
       </c>
-      <c r="S39" s="121">
+      <c r="S39" s="94">
         <f t="shared" si="25"/>
         <v>-0.13958333333333073</v>
       </c>
-      <c r="T39" s="122">
+      <c r="T39" s="95">
         <f t="shared" si="25"/>
         <v>-0.13958333333333073</v>
       </c>
@@ -11376,19 +11383,19 @@
         <v>2.5487500000000125</v>
       </c>
       <c r="P40" s="42"/>
-      <c r="Q40" s="120">
+      <c r="Q40" s="93">
         <f t="shared" ref="Q40:T40" si="28">Q30-G40</f>
         <v>-0.32458333333332945</v>
       </c>
-      <c r="R40" s="121">
+      <c r="R40" s="94">
         <f t="shared" si="28"/>
         <v>-0.32458333333332945</v>
       </c>
-      <c r="S40" s="121">
+      <c r="S40" s="94">
         <f t="shared" si="28"/>
         <v>-0.32458333333332945</v>
       </c>
-      <c r="T40" s="122">
+      <c r="T40" s="95">
         <f t="shared" si="28"/>
         <v>-0.32458333333332945</v>
       </c>
@@ -11411,41 +11418,41 @@
       </c>
     </row>
     <row r="42" spans="1:25" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B42" s="90" t="s">
+      <c r="B42" s="103" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="90"/>
-      <c r="D42" s="90"/>
-      <c r="E42" s="90"/>
+      <c r="C42" s="103"/>
+      <c r="D42" s="103"/>
+      <c r="E42" s="103"/>
       <c r="F42" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G42" s="90"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="90"/>
-      <c r="J42" s="90"/>
+      <c r="G42" s="103"/>
+      <c r="H42" s="103"/>
+      <c r="I42" s="103"/>
+      <c r="J42" s="103"/>
       <c r="K42" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L42" s="130"/>
-      <c r="M42" s="130"/>
-      <c r="N42" s="130"/>
-      <c r="O42" s="130"/>
+      <c r="L42" s="102"/>
+      <c r="M42" s="102"/>
+      <c r="N42" s="102"/>
+      <c r="O42" s="102"/>
       <c r="P42" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q42" s="130"/>
-      <c r="R42" s="130"/>
-      <c r="S42" s="130"/>
-      <c r="T42" s="130"/>
+      <c r="Q42" s="102"/>
+      <c r="R42" s="102"/>
+      <c r="S42" s="102"/>
+      <c r="T42" s="102"/>
       <c r="U42" s="51"/>
-      <c r="V42" s="130"/>
-      <c r="W42" s="130"/>
+      <c r="V42" s="102"/>
+      <c r="W42" s="102"/>
       <c r="X42"/>
-      <c r="Y42" s="130"/>
+      <c r="Y42" s="102"/>
     </row>
     <row r="43" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="I43" s="129"/>
+      <c r="I43" s="101"/>
       <c r="M43"/>
       <c r="S43"/>
     </row>
@@ -11456,26 +11463,26 @@
       <c r="M44"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L45" s="91" t="s">
+      <c r="L45" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="M45" s="91"/>
-      <c r="N45" s="91"/>
-      <c r="O45" s="91"/>
+      <c r="M45" s="105"/>
+      <c r="N45" s="105"/>
+      <c r="O45" s="105"/>
     </row>
     <row r="46" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="91" t="s">
+      <c r="B46" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="104"/>
-      <c r="D46" s="104"/>
-      <c r="E46" s="104"/>
-      <c r="G46" s="110" t="s">
+      <c r="C46" s="111"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="111"/>
+      <c r="G46" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H46" s="110"/>
-      <c r="I46" s="110"/>
-      <c r="J46" s="110"/>
+      <c r="H46" s="124"/>
+      <c r="I46" s="124"/>
+      <c r="J46" s="124"/>
       <c r="L46" s="12" t="s">
         <v>154</v>
       </c>
@@ -11488,18 +11495,18 @@
       <c r="O46" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="Q46" s="110" t="s">
+      <c r="Q46" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="R46" s="110"/>
-      <c r="S46" s="110"/>
-      <c r="T46" s="110"/>
-      <c r="V46" s="110" t="s">
+      <c r="R46" s="124"/>
+      <c r="S46" s="124"/>
+      <c r="T46" s="124"/>
+      <c r="V46" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="W46" s="110"/>
-      <c r="X46" s="110"/>
-      <c r="Y46" s="110"/>
+      <c r="W46" s="124"/>
+      <c r="X46" s="124"/>
+      <c r="Y46" s="124"/>
     </row>
     <row r="47" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="46">
@@ -11551,19 +11558,19 @@
         <v>6.4961265625000637</v>
       </c>
       <c r="P47" s="42"/>
-      <c r="Q47" s="120">
+      <c r="Q47" s="93">
         <f t="shared" ref="Q47:T47" si="33">Q35*Q35</f>
         <v>0.72604600694443755</v>
       </c>
-      <c r="R47" s="121">
+      <c r="R47" s="94">
         <f t="shared" si="33"/>
         <v>0.72604600694443755</v>
       </c>
-      <c r="S47" s="121">
+      <c r="S47" s="94">
         <f t="shared" si="33"/>
         <v>0.72604600694443755</v>
       </c>
-      <c r="T47" s="122">
+      <c r="T47" s="95">
         <f t="shared" si="33"/>
         <v>0.72604600694443755</v>
       </c>
@@ -11635,19 +11642,19 @@
         <v>6.4961265625000637</v>
       </c>
       <c r="P48" s="42"/>
-      <c r="Q48" s="120">
+      <c r="Q48" s="93">
         <f t="shared" ref="Q48:T48" si="38">Q36*Q36</f>
         <v>0.27257100694444203</v>
       </c>
-      <c r="R48" s="121">
+      <c r="R48" s="94">
         <f t="shared" si="38"/>
         <v>0.27257100694444203</v>
       </c>
-      <c r="S48" s="121">
+      <c r="S48" s="94">
         <f t="shared" si="38"/>
         <v>0.27257100694444203</v>
       </c>
-      <c r="T48" s="122">
+      <c r="T48" s="95">
         <f t="shared" si="38"/>
         <v>0.27257100694444203</v>
       </c>
@@ -11721,19 +11728,19 @@
         <v>6.4961265625000637</v>
       </c>
       <c r="P49" s="25"/>
-      <c r="Q49" s="120">
+      <c r="Q49" s="93">
         <f t="shared" ref="Q49:T49" si="43">Q37*Q37</f>
         <v>3.4425710069444446</v>
       </c>
-      <c r="R49" s="121">
+      <c r="R49" s="94">
         <f t="shared" si="43"/>
         <v>3.4425710069444446</v>
       </c>
-      <c r="S49" s="121">
+      <c r="S49" s="94">
         <f t="shared" si="43"/>
         <v>3.4425710069444446</v>
       </c>
-      <c r="T49" s="122">
+      <c r="T49" s="95">
         <f t="shared" si="43"/>
         <v>3.4425710069444446</v>
       </c>
@@ -11805,19 +11812,19 @@
         <v>6.4961265625000637</v>
       </c>
       <c r="P50" s="42"/>
-      <c r="Q50" s="120">
+      <c r="Q50" s="93">
         <f t="shared" ref="Q50:T50" si="48">Q38*Q38</f>
         <v>2.9184027777761105E-4</v>
       </c>
-      <c r="R50" s="121">
+      <c r="R50" s="94">
         <f t="shared" si="48"/>
         <v>2.9184027777761105E-4</v>
       </c>
-      <c r="S50" s="121">
+      <c r="S50" s="94">
         <f t="shared" si="48"/>
         <v>2.9184027777761105E-4</v>
       </c>
-      <c r="T50" s="122">
+      <c r="T50" s="95">
         <f t="shared" si="48"/>
         <v>2.9184027777761105E-4</v>
       </c>
@@ -11889,19 +11896,19 @@
         <v>6.4961265625000637</v>
       </c>
       <c r="P51" s="42"/>
-      <c r="Q51" s="120">
+      <c r="Q51" s="93">
         <f t="shared" ref="Q51:T51" si="53">Q39*Q39</f>
         <v>1.9483506944443719E-2</v>
       </c>
-      <c r="R51" s="121">
+      <c r="R51" s="94">
         <f t="shared" si="53"/>
         <v>1.9483506944443719E-2</v>
       </c>
-      <c r="S51" s="121">
+      <c r="S51" s="94">
         <f t="shared" si="53"/>
         <v>1.9483506944443719E-2</v>
       </c>
-      <c r="T51" s="122">
+      <c r="T51" s="95">
         <f t="shared" si="53"/>
         <v>1.9483506944443719E-2</v>
       </c>
@@ -11973,19 +11980,19 @@
         <v>6.4961265625000637</v>
       </c>
       <c r="P52" s="42"/>
-      <c r="Q52" s="120">
+      <c r="Q52" s="93">
         <f t="shared" ref="Q52:T52" si="58">Q40*Q40</f>
         <v>0.10535434027777525</v>
       </c>
-      <c r="R52" s="121">
+      <c r="R52" s="94">
         <f t="shared" si="58"/>
         <v>0.10535434027777525</v>
       </c>
-      <c r="S52" s="121">
+      <c r="S52" s="94">
         <f t="shared" si="58"/>
         <v>0.10535434027777525</v>
       </c>
-      <c r="T52" s="122">
+      <c r="T52" s="95">
         <f t="shared" si="58"/>
         <v>0.10535434027777525</v>
       </c>
@@ -12009,6 +12016,39 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="G3:J8"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="M3:M8"/>
+    <mergeCell ref="N3:N8"/>
+    <mergeCell ref="O3:O8"/>
+    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="G14:J19"/>
+    <mergeCell ref="L14:L19"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="M14:M19"/>
+    <mergeCell ref="N14:N19"/>
+    <mergeCell ref="O14:O19"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="V24:Y24"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="Q34:T34"/>
+    <mergeCell ref="V34:Y34"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="G46:J46"/>
     <mergeCell ref="Q46:T46"/>
@@ -12016,39 +12056,6 @@
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="G42:J42"/>
     <mergeCell ref="L45:O45"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="Q34:T34"/>
-    <mergeCell ref="V34:Y34"/>
-    <mergeCell ref="M14:M19"/>
-    <mergeCell ref="N14:N19"/>
-    <mergeCell ref="O14:O19"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="V13:Y13"/>
-    <mergeCell ref="G14:J19"/>
-    <mergeCell ref="L14:L19"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="V10:Y10"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="G3:J8"/>
-    <mergeCell ref="L3:L8"/>
-    <mergeCell ref="M3:M8"/>
-    <mergeCell ref="N3:N8"/>
-    <mergeCell ref="O3:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12070,12 +12077,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="12" t="s">
@@ -12092,7 +12099,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="127" t="s">
         <v>152</v>
       </c>
       <c r="C4" s="43">
@@ -12109,7 +12116,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="113"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="44">
         <v>24.21</v>
       </c>
@@ -12124,7 +12131,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="114"/>
+      <c r="B6" s="128"/>
       <c r="C6" s="45">
         <v>26.88</v>
       </c>
@@ -12139,7 +12146,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="127" t="s">
         <v>153</v>
       </c>
       <c r="C7" s="44">
@@ -12156,7 +12163,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="113"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="44">
         <v>23.4</v>
       </c>
@@ -12171,7 +12178,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="113"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="45">
         <v>23.35</v>
       </c>
@@ -12186,15 +12193,14 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="91" t="s">
+      <c r="C12" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="123"/>
       <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
@@ -12209,92 +12215,92 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="96" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="125">
+      <c r="C14" s="97">
         <v>19.12</v>
       </c>
-      <c r="D14" s="125">
+      <c r="D14" s="97">
         <v>18.559999999999999</v>
       </c>
-      <c r="E14" s="125">
+      <c r="E14" s="97">
         <v>25.58</v>
       </c>
-      <c r="F14" s="125">
+      <c r="F14" s="97">
         <v>24.39</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="100" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="126">
+      <c r="C15" s="98">
         <v>24.21</v>
       </c>
-      <c r="D15" s="126">
+      <c r="D15" s="98">
         <v>20</v>
       </c>
-      <c r="E15" s="126">
+      <c r="E15" s="98">
         <v>23.31</v>
       </c>
-      <c r="F15" s="126">
+      <c r="F15" s="98">
         <v>21.45</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="128" t="s">
+      <c r="B16" s="100" t="s">
         <v>168</v>
       </c>
-      <c r="C16" s="126">
+      <c r="C16" s="98">
         <v>26.88</v>
       </c>
-      <c r="D16" s="126">
+      <c r="D16" s="98">
         <v>19.87</v>
       </c>
-      <c r="E16" s="126">
+      <c r="E16" s="98">
         <v>18.989999999999998</v>
       </c>
-      <c r="F16" s="126">
+      <c r="F16" s="98">
         <v>32.74</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="127" t="s">
+      <c r="B17" s="99" t="s">
         <v>169</v>
       </c>
-      <c r="C17" s="126">
+      <c r="C17" s="98">
         <v>21.6</v>
       </c>
-      <c r="D17" s="126">
+      <c r="D17" s="98">
         <v>22.09</v>
       </c>
-      <c r="E17" s="126">
+      <c r="E17" s="98">
         <v>23.09</v>
       </c>
-      <c r="F17" s="126">
+      <c r="F17" s="98">
         <v>24.21</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="127" t="s">
+      <c r="B18" s="99" t="s">
         <v>170</v>
       </c>
-      <c r="C18" s="126">
+      <c r="C18" s="98">
         <v>23.4</v>
       </c>
-      <c r="D18" s="126">
+      <c r="D18" s="98">
         <v>17.62</v>
       </c>
-      <c r="E18" s="126">
+      <c r="E18" s="98">
         <v>23.81</v>
       </c>
-      <c r="F18" s="126">
+      <c r="F18" s="98">
         <v>25.67</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="124" t="s">
+      <c r="B19" s="96" t="s">
         <v>171</v>
       </c>
       <c r="C19" s="45">
@@ -12442,18 +12448,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="L2" s="91" t="s">
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="L2" s="105" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
     </row>
     <row r="3" spans="1:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="81" t="s">
@@ -12469,12 +12475,12 @@
         <v>148</v>
       </c>
       <c r="F3" s="78"/>
-      <c r="G3" s="110" t="s">
+      <c r="G3" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
       <c r="K3" s="78"/>
       <c r="L3" s="81" t="s">
         <v>145</v>
@@ -12728,18 +12734,18 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="L12" s="91" t="s">
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="L12" s="105" t="s">
         <v>150</v>
       </c>
-      <c r="M12" s="91"/>
-      <c r="N12" s="91"/>
-      <c r="O12" s="91"/>
+      <c r="M12" s="105"/>
+      <c r="N12" s="105"/>
+      <c r="O12" s="105"/>
     </row>
     <row r="13" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="81" t="s">
@@ -12755,12 +12761,12 @@
         <v>148</v>
       </c>
       <c r="F13" s="78"/>
-      <c r="G13" s="110" t="s">
+      <c r="G13" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="124"/>
       <c r="K13" s="78"/>
       <c r="L13" s="81" t="s">
         <v>145</v>
@@ -12775,12 +12781,12 @@
         <v>148</v>
       </c>
       <c r="P13" s="78"/>
-      <c r="Q13" s="110" t="s">
+      <c r="Q13" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="R13" s="110"/>
-      <c r="S13" s="110"/>
-      <c r="T13" s="110"/>
+      <c r="R13" s="124"/>
+      <c r="S13" s="124"/>
+      <c r="T13" s="124"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="46">
@@ -13068,18 +13074,18 @@
       <c r="T19" s="80"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="L22" s="91" t="s">
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="L22" s="105" t="s">
         <v>150</v>
       </c>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="91"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="105"/>
+      <c r="O22" s="105"/>
     </row>
     <row r="23" spans="2:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="81" t="s">
@@ -13095,12 +13101,12 @@
         <v>148</v>
       </c>
       <c r="F23" s="78"/>
-      <c r="G23" s="110" t="s">
+      <c r="G23" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
+      <c r="H23" s="124"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="124"/>
       <c r="K23" s="78"/>
       <c r="L23" s="81" t="s">
         <v>145</v>
@@ -13115,12 +13121,12 @@
         <v>148</v>
       </c>
       <c r="P23" s="78"/>
-      <c r="Q23" s="110" t="s">
+      <c r="Q23" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="R23" s="110"/>
-      <c r="S23" s="110"/>
-      <c r="T23" s="110"/>
+      <c r="R23" s="124"/>
+      <c r="S23" s="124"/>
+      <c r="T23" s="124"/>
     </row>
     <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="46">
@@ -13481,17 +13487,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="L12:O12"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="Q13:T13"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="L22:O22"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="L12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>